<commit_message>
correção pendencias nas iterações e ajuste caso de uso
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Projetos\GitHub\cmproject\planejamento\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de Itens de Trabalho" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Lista de Itens de Trabalho" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
-    <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -123,16 +127,13 @@
     <t>corrigir pendencias da iteração anterior</t>
   </si>
   <si>
-    <t>Não iniciado</t>
-  </si>
-  <si>
     <t>Refinar requisito selecionado</t>
   </si>
   <si>
     <t>Italo/Tarcísio</t>
   </si>
   <si>
-    <t>Criar novo plano de iteração </t>
+    <t>Criar novo plano de iteração</t>
   </si>
   <si>
     <t>atualizar riscos</t>
@@ -145,17 +146,16 @@
   </si>
   <si>
     <t>Caso de uso projetado</t>
+  </si>
+  <si>
+    <t>Iniciado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,33 +164,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Arial1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -198,15 +179,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -241,112 +213,54 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="12">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 1" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 1" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Canto da tabela dinâmica" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Valor da tabela dinâmica" xfId="25" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texto Explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -405,91 +319,361 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6511627906977"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3860465116279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1395348837209"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2558139534884"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4976744186046"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.37674418604651"/>
+    <col min="1" max="1" width="30.875"/>
+    <col min="2" max="2" width="13.5"/>
+    <col min="3" max="3" width="11.625"/>
+    <col min="4" max="4" width="10.75"/>
+    <col min="5" max="5" width="10.375"/>
+    <col min="6" max="6" width="11.125"/>
+    <col min="7" max="7" width="11.5"/>
+    <col min="8" max="8" width="10.25"/>
+    <col min="9" max="9" width="25.5"/>
+    <col min="10" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="38.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <f aca="false">G3</f>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3:C12" si="0">G3</f>
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -501,23 +685,23 @@
       <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="n">
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
         <v>1</v>
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <f aca="false">G4</f>
+      <c r="C4" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -529,25 +713,25 @@
       <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5" t="n">
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" ht="14.65" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="n">
-        <f aca="false">G5</f>
+      <c r="C5" s="5">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -559,23 +743,23 @@
       <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="5">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="5">
         <v>3</v>
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="14.65" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="n">
-        <f aca="false">G6</f>
+      <c r="C6" s="5">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -587,23 +771,23 @@
       <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="5">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="5">
         <v>1</v>
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="n">
-        <f aca="false">G7</f>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -615,23 +799,23 @@
       <c r="F7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="5">
         <v>3</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="5">
         <v>3</v>
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="n">
-        <f aca="false">G8</f>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -643,23 +827,23 @@
       <c r="F8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="5">
         <v>3</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="5">
         <v>2</v>
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5" t="n">
-        <f aca="false">G9</f>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -671,23 +855,23 @@
       <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="5">
         <v>6</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="5">
         <v>2</v>
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" ht="14.65" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5" t="n">
-        <f aca="false">G10</f>
+      <c r="C10" s="5">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -699,23 +883,23 @@
       <c r="F10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="5">
         <v>15</v>
       </c>
-      <c r="H10" s="5" t="n">
+      <c r="H10" s="5">
         <v>12</v>
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" ht="14.65" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5" t="n">
-        <f aca="false">G11</f>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -727,25 +911,25 @@
       <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="5">
         <v>20</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="5">
         <v>8</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="n">
-        <f aca="false">G12</f>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -757,22 +941,22 @@
       <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="5">
         <v>4</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="5">
         <v>5</v>
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="5">
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -784,35 +968,35 @@
       <c r="F13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="5" t="n">
+      <c r="G13" s="5">
+        <v>12</v>
+      </c>
+      <c r="H13" s="5">
         <v>11</v>
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="5">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -824,184 +1008,189 @@
       <c r="F15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="5" t="n">
-        <f aca="false">C15</f>
-        <v>1</v>
-      </c>
-      <c r="H15" s="5" t="n">
+      <c r="G15" s="5">
+        <f t="shared" ref="G15:G21" si="1">C15</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
         <v>1</v>
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="5">
         <v>6</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="5" t="n">
-        <f aca="false">C16</f>
+        <v>35</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="6">
+        <v>7</v>
+      </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="0" t="n">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>34</v>
+      <c r="D17" t="s">
+        <v>41</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="5" t="n">
-        <f aca="false">C17</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="5" t="n">
-        <f aca="false">C18</f>
-        <v>1</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="5" t="n">
-        <f aca="false">C19</f>
-        <v>1</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="0" t="n">
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="H20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="5" t="n">
-        <f aca="false">C20</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="0" t="n">
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="5" t="n">
-        <f aca="false">C21</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.65" customHeight="1"/>
+    <row r="25" spans="1:8" ht="14.65" customHeight="1"/>
+    <row r="36" ht="14.65" customHeight="1"/>
+    <row r="37" ht="14.65" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:I25"/>
   <mergeCells count="2">
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A14:I14"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="1.27916666666667" bottom="1.27916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="1.2791666666666699" bottom="1.2791666666666699" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finalização plano iteração elaboração
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -14,13 +14,14 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -137,9 +138,6 @@
   </si>
   <si>
     <t>Analise e projeto do caso de uso</t>
-  </si>
-  <si>
-    <t>Iniciado</t>
   </si>
   <si>
     <t>E2</t>
@@ -370,8 +368,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -902,10 +900,10 @@
         <v>10</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>34</v>
@@ -915,12 +913,12 @@
         <v>10</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>11</v>
@@ -929,10 +927,10 @@
         <v>30</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>34</v>
@@ -942,9 +940,10 @@
         <v>30</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Criação de novo plano de iteração
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Itens de Trabalho" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,13 +15,15 @@
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -144,6 +146,33 @@
   </si>
   <si>
     <t>Caso de uso projetado</t>
+  </si>
+  <si>
+    <t>Elaboração 2</t>
+  </si>
+  <si>
+    <t>Adicionar integrante ao repositório</t>
+  </si>
+  <si>
+    <t>Não Iniciado</t>
+  </si>
+  <si>
+    <t>Correções de erros da etapa anterior</t>
+  </si>
+  <si>
+    <t>Tarcísio/ Diógenes</t>
+  </si>
+  <si>
+    <t>Configuração ambiente do novo integrante</t>
+  </si>
+  <si>
+    <t>Diógenes</t>
+  </si>
+  <si>
+    <t>Atualizar artefatos</t>
+  </si>
+  <si>
+    <t>Lições aprendidas</t>
   </si>
 </sst>
 </file>
@@ -368,22 +397,22 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5023255813954"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6232558139535"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3767441860465"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1255813953488"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5023255813954"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2558139534884"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4976744186046"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.37674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.9488372093023"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -943,16 +972,157 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:I25"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A22:I22"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="1.27916666666667" bottom="1.27916666666667" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
update marcos para iteração ³
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -18,13 +18,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -176,7 +177,7 @@
     <t>Refinar requisitos</t>
   </si>
   <si>
-    <t>Atualizar diagramas UML </t>
+    <t>Atualizar diagramas UML</t>
   </si>
   <si>
     <t>alta</t>
@@ -189,6 +190,12 @@
   </si>
   <si>
     <t>Testar aplicação</t>
+  </si>
+  <si>
+    <t>implementar os casos de uso selecionados para a iteração</t>
+  </si>
+  <si>
+    <t>Iniciado</t>
   </si>
 </sst>
 </file>
@@ -414,7 +421,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1235,6 +1242,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
update formatação e fonte ²
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="927" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Itens de Trabalho" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -229,19 +230,18 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -317,24 +317,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -420,851 +420,840 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2279069767442"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.9488372093023"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.5953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.2"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="n">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <f aca="false">G3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">G4</f>
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="G4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="n">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <f aca="false">G5</f>
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="n">
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <f aca="false">G6</f>
         <v>2</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="n">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <f aca="false">G7</f>
         <v>3</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="n">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <f aca="false">G8</f>
         <v>3</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="5" t="n">
+      <c r="H8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5" t="n">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <f aca="false">G9</f>
         <v>6</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="n">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <f aca="false">G10</f>
         <v>15</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H10" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="I10" s="5"/>
+      <c r="H10" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">G11</f>
         <v>20</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="H11" s="5" t="n">
+      <c r="H11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="1" t="n">
         <f aca="false">G12</f>
         <v>4</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H12" s="5" t="n">
+      <c r="H12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="I13" s="5"/>
+      <c r="G13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="1" t="n">
         <f aca="false">C15</f>
         <v>1</v>
       </c>
-      <c r="H15" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5"/>
+      <c r="H15" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="5" t="n">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="1" t="n">
         <f aca="false">C16</f>
         <v>6</v>
       </c>
-      <c r="H16" s="5" t="n">
+      <c r="H16" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="0" t="n">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="1" t="n">
         <f aca="false">C17</f>
         <v>4</v>
       </c>
-      <c r="H17" s="5" t="n">
+      <c r="H17" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="1" t="n">
         <f aca="false">C18</f>
         <v>1</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="1" t="n">
         <f aca="false">C19</f>
         <v>1</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="0" t="n">
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="1" t="n">
         <f aca="false">C20</f>
         <v>10</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="0" t="n">
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="1" t="n">
         <f aca="false">C21</f>
         <v>30</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="0" t="n">
+      <c r="G23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="0" t="n">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="0" t="n">
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="D25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="0" t="n">
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="D26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="0" t="n">
+      <c r="B27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="D27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="0" t="n">
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="1" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="0" t="s">
+      <c r="E29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="0" t="s">
+      <c r="E30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="0" t="n">
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="0" t="n">
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualização de horas trabalhadas nos itens do projeto
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Itens de Trabalho" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,6 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -184,19 +185,19 @@
     <t>alta</t>
   </si>
   <si>
+    <t>Iniciado</t>
+  </si>
+  <si>
+    <t>Construir diagramas dos demais casos de uso</t>
+  </si>
+  <si>
+    <t>Testar aplicação</t>
+  </si>
+  <si>
     <t>Não iniciado</t>
   </si>
   <si>
-    <t>Construir diagramas dos demais casos de uso</t>
-  </si>
-  <si>
-    <t>Testar aplicação</t>
-  </si>
-  <si>
     <t>implementar os casos de uso selecionados para a iteração</t>
-  </si>
-  <si>
-    <t>Iniciado</t>
   </si>
 </sst>
 </file>
@@ -230,6 +231,7 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -237,7 +239,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -312,29 +313,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -420,22 +425,22 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.5953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.2"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.8139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -481,306 +486,315 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <f aca="false">G3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="G3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="6" t="n">
         <f aca="false">G4</f>
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="G4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="n">
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="n">
         <f aca="false">G5</f>
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="6" t="n">
         <v>3</v>
       </c>
+      <c r="I5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="n">
         <f aca="false">G6</f>
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="H6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="n">
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="n">
         <f aca="false">G7</f>
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="6" t="n">
         <v>3</v>
       </c>
+      <c r="I7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="n">
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="n">
         <f aca="false">G8</f>
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="6" t="n">
         <v>2</v>
       </c>
+      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="n">
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="n">
         <f aca="false">G9</f>
         <v>6</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="6" t="n">
         <v>2</v>
       </c>
+      <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="n">
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="n">
         <f aca="false">G10</f>
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="H10" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="H10" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="6" t="n">
         <f aca="false">G11</f>
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="G11" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="6" t="n">
         <f aca="false">G12</f>
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="H12" s="1" t="n">
+      <c r="H12" s="6" t="n">
         <v>5</v>
       </c>
+      <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="G13" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -796,193 +810,200 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="6" t="n">
         <f aca="false">C15</f>
         <v>1</v>
       </c>
-      <c r="H15" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="H15" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="n">
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="D16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G16" s="6" t="n">
         <f aca="false">C16</f>
         <v>6</v>
       </c>
-      <c r="H16" s="1" t="n">
+      <c r="H16" s="6" t="n">
         <v>7</v>
       </c>
+      <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="n">
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="G17" s="6" t="n">
         <f aca="false">C17</f>
         <v>4</v>
       </c>
-      <c r="H17" s="1" t="n">
+      <c r="H17" s="6" t="n">
         <v>3</v>
       </c>
+      <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="G18" s="6" t="n">
         <f aca="false">C18</f>
         <v>1</v>
       </c>
-      <c r="H18" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="H18" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="C19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="G19" s="6" t="n">
         <f aca="false">C19</f>
         <v>1</v>
       </c>
-      <c r="H19" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="H19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1" t="n">
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="6" t="n">
         <f aca="false">C20</f>
         <v>10</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="6" t="n">
         <v>10</v>
       </c>
+      <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="n">
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="6" t="n">
         <v>30</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="G21" s="6" t="n">
         <f aca="false">C21</f>
         <v>30</v>
       </c>
-      <c r="H21" s="1" t="n">
-        <v>32</v>
-      </c>
+      <c r="H21" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
@@ -998,263 +1019,263 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="B23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1" t="n">
+      <c r="G23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1" t="n">
+      <c r="B24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="D24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="G24" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="6" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="1" t="n">
+      <c r="B25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="D25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="G25" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="H25" s="1" t="n">
+      <c r="H25" s="6" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="n">
+      <c r="B26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="D26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="H26" s="1" t="n">
+      <c r="H26" s="6" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="1" t="n">
+      <c r="B27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="D27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="G27" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="H27" s="1" t="n">
+      <c r="H27" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="1" t="n">
+      <c r="B28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="D28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="G28" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="H28" s="1" t="n">
+      <c r="H28" s="6" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="E29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="G29" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="H29" s="1" t="n">
+      <c r="H29" s="6" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="G30" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H30" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H31" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="6" t="n">
+        <v>70</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G31" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="1" t="n">
+      <c r="G32" s="6" t="n">
         <v>60</v>
       </c>
-      <c r="H32" s="1" t="n">
-        <v>15</v>
+      <c r="H32" s="6" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Planejamento para nova etapa - Construção 1
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="62">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>Elaboração I</t>
+  </si>
+  <si>
+    <t>Construção 1</t>
+  </si>
+  <si>
+    <t>Implementar os casos de uso funcional</t>
+  </si>
+  <si>
+    <t>Cumprir todos os requisitos do produto definidos na visão</t>
+  </si>
+  <si>
+    <t>Corrigir inconsistências dos diagramas UML</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Baixa</t>
   </si>
 </sst>
 </file>
@@ -228,7 +246,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +269,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF99FF33"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF47CD27"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -279,19 +303,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -314,6 +349,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -331,6 +367,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -348,6 +385,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -365,6 +403,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -382,6 +421,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -399,6 +439,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -416,6 +457,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -433,6 +475,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -450,6 +493,14 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -474,13 +525,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -585,6 +630,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF47CD27"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -598,7 +646,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:I43" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:I43" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
   <autoFilter ref="A1:I43"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Nome / Descrição" dataDxfId="8"/>
@@ -878,19 +926,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK38"/>
+  <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1"/>
     <col min="3" max="3" width="11.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.125" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
     <col min="9" max="9" width="28.625" style="1"/>
@@ -898,842 +947,1053 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6">
         <f t="shared" ref="C3:C12" si="0">G3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="6">
         <v>2</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="6">
         <v>3</v>
       </c>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>2</v>
       </c>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="6">
         <v>3</v>
       </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="6">
         <v>3</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="6">
         <v>2</v>
       </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="6">
         <v>6</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="6">
         <v>2</v>
       </c>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="6">
         <v>15</v>
       </c>
-      <c r="H10" s="3">
-        <v>12</v>
-      </c>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="H10" s="6">
+        <v>12</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <v>20</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="6">
         <v>8</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="6">
         <v>4</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="6">
         <v>5</v>
       </c>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="3">
-        <v>12</v>
-      </c>
-      <c r="H13" s="3">
-        <v>11</v>
-      </c>
-      <c r="I13"/>
+      <c r="G13" s="6">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6">
+        <v>11</v>
+      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="6">
         <f t="shared" ref="G15:G21" si="1">C15</f>
         <v>1</v>
       </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6">
         <v>6</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="6">
         <v>7</v>
       </c>
-      <c r="I16"/>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="6">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="6">
         <v>3</v>
       </c>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H18" s="3">
-        <v>1</v>
-      </c>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="6">
         <v>10</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="6">
         <v>10</v>
       </c>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="6">
         <v>30</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="6">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="6">
         <v>32</v>
       </c>
-      <c r="I21"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="B23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="3">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3">
+      <c r="B24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="6">
         <v>10</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="6">
         <v>10</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="3">
+      <c r="B25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="6">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="6">
         <v>2</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="B26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="6">
         <v>15</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="6">
         <v>15</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="B27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="6">
         <v>2</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="6">
         <v>2</v>
       </c>
-      <c r="H27" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="H27" s="6">
+        <v>1</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="3">
+      <c r="B28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="6">
         <v>8</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="6">
         <v>9</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="3">
+      <c r="B29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="6">
         <v>7</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="6">
         <v>7</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="6">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="3">
+      <c r="B30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="6">
         <v>10</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="6">
         <v>10</v>
       </c>
-      <c r="H30" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="H30" s="6">
+        <v>12</v>
+      </c>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="3">
+      <c r="B31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="6">
         <v>6</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="6">
         <v>6</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="3">
+      <c r="B32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="6">
         <v>70</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="6">
         <v>60</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="6">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="6">
+        <v>25</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="6">
+        <v>25</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="8">
+        <v>10</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="8">
+        <v>10</v>
+      </c>
+      <c r="H35" s="8">
+        <v>0</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="8">
+        <v>70</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="8">
+        <v>70</v>
+      </c>
+      <c r="H36" s="8">
+        <v>0</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="8">
+        <v>12</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="8">
+        <v>12</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="8">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G38" s="8">
+        <v>5</v>
+      </c>
+      <c r="H38" s="8">
+        <v>0</v>
+      </c>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="1.2791666666666699" bottom="1.2791666666666699" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
plano de iteracao Construção I
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -497,13 +497,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -526,6 +519,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -646,7 +646,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:I43" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:I43" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A1:I43"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Nome / Descrição" dataDxfId="8"/>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1804,7 +1804,7 @@
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
update lista item iteração
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarcisio.d.silva\Documents\GitHub\cmproject\cmproject.git\planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\cmproject\planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="753"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Itens de Trabalho" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Lista de Itens de Trabalho'!$A$1:$I$25</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,7 +666,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -704,7 +704,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -776,7 +776,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -940,8 +940,8 @@
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="28.625" style="1"/>
     <col min="10" max="1025" width="9.375" style="1"/>
   </cols>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>49</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>25</v>
       </c>
       <c r="H34" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I34" s="6"/>
     </row>
@@ -1842,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>13</v>
@@ -1854,11 +1854,11 @@
         <v>10</v>
       </c>
       <c r="H35" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>57</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>70</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>13</v>
@@ -1881,7 +1881,7 @@
         <v>70</v>
       </c>
       <c r="H36" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I36" s="8"/>
     </row>
@@ -1896,7 +1896,7 @@
         <v>12</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>13</v>
@@ -1908,7 +1908,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="8"/>
     </row>
@@ -1935,7 +1935,7 @@
         <v>5</v>
       </c>
       <c r="H38" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I38" s="8"/>
     </row>

</xml_diff>

<commit_message>
Update de lista de itens
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_Itens.xlsx
+++ b/planejamento/CM_Lista_Itens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\cmproject\planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Github\cmproject\planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -929,17 +929,17 @@
   <dimension ref="A1:AMK43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1"/>
     <col min="3" max="3" width="11.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.75" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="16.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="28.625" style="1"/>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="I25" s="8"/>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="I28" s="8"/>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>49</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>52</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>42</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>25</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>13</v>
@@ -1842,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>13</v>
@@ -1881,7 +1881,7 @@
         <v>70</v>
       </c>
       <c r="H36" s="8">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="I36" s="8"/>
     </row>
@@ -1896,7 +1896,7 @@
         <v>12</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>13</v>
@@ -1908,7 +1908,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I37" s="8"/>
     </row>
@@ -1923,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>13</v>
@@ -1935,7 +1935,7 @@
         <v>5</v>
       </c>
       <c r="H38" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I38" s="8"/>
     </row>

</xml_diff>